<commit_message>
Mean + error fixes
</commit_message>
<xml_diff>
--- a/Error Rates.xlsx
+++ b/Error Rates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="11340" windowHeight="9855"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="16140" windowHeight="6285"/>
   </bookViews>
   <sheets>
     <sheet name="Error Rates" sheetId="1" r:id="rId1"/>
@@ -14,21 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>354 samples : No preprocessing</t>
-  </si>
-  <si>
-    <t>Nr of Hidden Nodes</t>
-  </si>
-  <si>
-    <t>Nr of training epochs</t>
-  </si>
-  <si>
-    <t>TrainError</t>
-  </si>
-  <si>
-    <t>TestError</t>
+    <t>Dimensie 81</t>
   </si>
 </sst>
 </file>
@@ -513,9 +501,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -581,13 +568,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="nl-BE"/>
-              <a:t>Error rates with 354 samples no preprocessing</a:t>
+              <a:t>TrainingsError</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="1"/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -598,11 +584,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Error Rates'!$C$2</c:f>
+              <c:f>'Error Rates'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TrainError</c:v>
+                  <c:v>0,1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -614,10 +600,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>'Error Rates'!$A$3:$A$7</c:f>
+              <c:f>'Error Rates'!$B$4:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -625,37 +611,43 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>200</c:v>
+                <c:pt idx="5">
+                  <c:v>120</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Error Rates'!$C$3:$C$7</c:f>
+              <c:f>('Error Rates'!$E$1,'Error Rates'!$E$5,'Error Rates'!$E$9,'Error Rates'!$E$13,'Error Rates'!$E$17,'Error Rates'!$E$21)</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>48.120300751899997</c:v>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>44.509554140100001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>47.744360902300002</c:v>
+                  <c:v>41.019108280300003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.375939849600002</c:v>
+                  <c:v>39.974522293</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>48.120300751899997</c:v>
+                  <c:v>39.503184713400003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43.984962406000001</c:v>
+                  <c:v>40.369426751600002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40.828025477700002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -670,7 +662,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TestError</c:v>
+                  <c:v>0,01</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -682,10 +674,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>'Error Rates'!$A$3:$A$7</c:f>
+              <c:f>'Error Rates'!$B$4:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -693,47 +685,201 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>200</c:v>
+                <c:pt idx="5">
+                  <c:v>120</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Error Rates'!$D$3:$D$7</c:f>
+              <c:f>('Error Rates'!$E$2,'Error Rates'!$E$6,'Error Rates'!$E$10,'Error Rates'!$E$14,'Error Rates'!$E$18,'Error Rates'!$E$22)</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>51.136363636399999</c:v>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>35.197452229299998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40.909090909100001</c:v>
+                  <c:v>31.273885350299999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53.409090909100001</c:v>
+                  <c:v>27.949044585999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43.181818181799997</c:v>
+                  <c:v>27.707006369399998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55.681818181799997</c:v>
+                  <c:v>26.407643312099999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26.535031847100001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="42891904"/>
-        <c:axId val="124731392"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Error Rates'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0,001</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Error Rates'!$B$4:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Error Rates'!$E$3,'Error Rates'!$E$7,'Error Rates'!$E$11,'Error Rates'!$E$15,'Error Rates'!$E$19,'Error Rates'!$E$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>36.573248407599998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.152866242000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.203821656100001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.407643312099999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.605095541400001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27.031847133799999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Error Rates'!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0,0001</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Error Rates'!$B$4:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Error Rates'!$E$4,'Error Rates'!$E$8,'Error Rates'!$E$16,'Error Rates'!$E$12,'Error Rates'!$E$24,'Error Rates'!$E$20)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>37.3503184713</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31.9872611465</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.025477707</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.4968152866</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26.560509554100001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.356687898099999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="90123264"/>
+        <c:axId val="60577280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42891904"/>
+        <c:axId val="90123264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -758,15 +904,15 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124731392"/>
+        <c:crossAx val="60577280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="124731392"/>
+        <c:axId val="60577280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="40"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
@@ -781,16 +927,16 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="nl-BE"/>
-                  <a:t>Error rate (%)</a:t>
+                  <a:t>Error rate</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:layout/>
         </c:title>
-        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42891904"/>
+        <c:crossAx val="90123264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -803,7 +949,415 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="nl-BE"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-BE"/>
+              <a:t>TestError</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Error Rates'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0,1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Error Rates'!$B$4:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Error Rates'!$F$1,'Error Rates'!$F$5,'Error Rates'!$F$9,'Error Rates'!$F$13,'Error Rates'!$F$17,'Error Rates'!$F$21)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>46.961538461499998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50.961538461499998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49.7307692308</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46.7692307692</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48.076923076900002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50.153846153800004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Error Rates'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0,01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Error Rates'!$B$4:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Error Rates'!$F$2,'Error Rates'!$F$6,'Error Rates'!$F$10,'Error Rates'!$F$14,'Error Rates'!$F$18,'Error Rates'!$F$22)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>48.923076923099998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48.192307692299998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49.653846153800004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45.461538461499998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46.7692307692</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Error Rates'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0,001</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Error Rates'!$B$4:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Error Rates'!$F$3,'Error Rates'!$F$7,'Error Rates'!$F$11,'Error Rates'!$F$15,'Error Rates'!$F$19,'Error Rates'!$F$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>49.653846153800004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46.2307692308</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51.076923076900002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47.384615384600004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47.7692307692</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>49.115384615400004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Error Rates'!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0,0001</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Error Rates'!$B$4:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Error Rates'!$F$4,'Error Rates'!$F$8,'Error Rates'!$F$12,'Error Rates'!$F$16,'Error Rates'!$F$21,'Error Rates'!$F$20,'Error Rates'!$F$21,'Error Rates'!$F$24)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>47.653846153800004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>47.076923076900002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46.038461538500002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47.384615384600004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.153846153800004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45.115384615400004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50.153846153800004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>48.538461538500002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="60616704"/>
+        <c:axId val="60618624"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="60616704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-BE"/>
+                  <a:t>Nr of hidden nodes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="60618624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="60618624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-BE"/>
+                  <a:t>Error rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="60616704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -813,16 +1367,46 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafiek 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -835,7 +1419,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1129,135 +1713,372 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
+      <c r="C1">
         <v>20</v>
       </c>
-      <c r="B3">
-        <v>100</v>
-      </c>
-      <c r="C3" s="1">
-        <v>48.120300751899997</v>
-      </c>
-      <c r="D3" s="1">
-        <v>51.136363636399999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
+      <c r="D1">
+        <v>0.1</v>
+      </c>
+      <c r="E1">
+        <v>44.509554140100001</v>
+      </c>
+      <c r="F1">
+        <v>46.961538461499998</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>0.01</v>
+      </c>
+      <c r="E2">
+        <v>35.197452229299998</v>
+      </c>
+      <c r="F2">
+        <v>48.923076923099998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>1E-3</v>
+      </c>
+      <c r="E3">
+        <v>36.573248407599998</v>
+      </c>
+      <c r="F3">
+        <v>49.653846153800004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>1E-4</v>
+      </c>
+      <c r="E4">
+        <v>37.3503184713</v>
+      </c>
+      <c r="F4">
+        <v>47.653846153800004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="B5">
         <v>40</v>
       </c>
-      <c r="B4">
-        <v>100</v>
-      </c>
-      <c r="C4" s="1">
-        <v>47.744360902300002</v>
-      </c>
-      <c r="D4" s="1">
-        <v>40.909090909100001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
+      <c r="C5">
+        <v>40</v>
+      </c>
+      <c r="D5">
+        <v>0.1</v>
+      </c>
+      <c r="E5">
+        <v>41.019108280300003</v>
+      </c>
+      <c r="F5">
+        <v>50.961538461499998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="B6">
+        <v>60</v>
+      </c>
+      <c r="C6">
+        <v>40</v>
+      </c>
+      <c r="D6">
+        <v>0.01</v>
+      </c>
+      <c r="E6">
+        <v>31.273885350299999</v>
+      </c>
+      <c r="F6">
+        <v>48.192307692299998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7">
         <v>80</v>
       </c>
-      <c r="B5">
-        <v>100</v>
-      </c>
-      <c r="C5" s="1">
-        <v>50.375939849600002</v>
-      </c>
-      <c r="D5" s="1">
-        <v>53.409090909100001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>100</v>
-      </c>
-      <c r="B6">
-        <v>100</v>
-      </c>
-      <c r="C6" s="1">
-        <v>48.120300751899997</v>
-      </c>
-      <c r="D6" s="1">
-        <v>43.181818181799997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>200</v>
-      </c>
-      <c r="B7">
-        <v>100</v>
-      </c>
-      <c r="C7" s="1">
-        <v>43.984962406000001</v>
-      </c>
-      <c r="D7" s="1">
-        <v>55.681818181799997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>500</v>
-      </c>
+      <c r="C7">
+        <v>40</v>
+      </c>
+      <c r="D7">
+        <v>1E-3</v>
+      </c>
+      <c r="E7">
+        <v>32.152866242000002</v>
+      </c>
+      <c r="F7">
+        <v>46.2307692308</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="B8">
         <v>100</v>
       </c>
-      <c r="C8" s="1">
-        <v>49.624060150399998</v>
-      </c>
-      <c r="D8" s="1">
-        <v>53.409090909100001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>1000</v>
-      </c>
+      <c r="C8">
+        <v>40</v>
+      </c>
+      <c r="D8">
+        <v>1E-4</v>
+      </c>
+      <c r="E8">
+        <v>31.9872611465</v>
+      </c>
+      <c r="F8">
+        <v>47.076923076900002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="B9">
+        <v>120</v>
+      </c>
+      <c r="C9">
+        <v>60</v>
+      </c>
+      <c r="D9">
+        <v>0.1</v>
+      </c>
+      <c r="E9">
+        <v>39.974522293</v>
+      </c>
+      <c r="F9">
+        <v>49.7307692308</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="C10">
+        <v>60</v>
+      </c>
+      <c r="D10">
+        <v>0.01</v>
+      </c>
+      <c r="E10">
+        <v>27.949044585999999</v>
+      </c>
+      <c r="F10">
+        <v>49.653846153800004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="C11">
+        <v>60</v>
+      </c>
+      <c r="D11">
+        <v>1E-3</v>
+      </c>
+      <c r="E11">
+        <v>30.203821656100001</v>
+      </c>
+      <c r="F11">
+        <v>51.076923076900002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="C12">
+        <v>60</v>
+      </c>
+      <c r="D12">
+        <v>1E-4</v>
+      </c>
+      <c r="E12">
+        <v>30.4968152866</v>
+      </c>
+      <c r="F12">
+        <v>46.038461538500002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="C13">
+        <v>80</v>
+      </c>
+      <c r="D13">
+        <v>0.1</v>
+      </c>
+      <c r="E13">
+        <v>39.503184713400003</v>
+      </c>
+      <c r="F13">
+        <v>46.7692307692</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="C14">
+        <v>80</v>
+      </c>
+      <c r="D14">
+        <v>0.01</v>
+      </c>
+      <c r="E14">
+        <v>27.707006369399998</v>
+      </c>
+      <c r="F14">
+        <v>45.461538461499998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="C15">
+        <v>80</v>
+      </c>
+      <c r="D15">
+        <v>1E-3</v>
+      </c>
+      <c r="E15">
+        <v>26.407643312099999</v>
+      </c>
+      <c r="F15">
+        <v>47.384615384600004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="C16">
+        <v>80</v>
+      </c>
+      <c r="D16">
+        <v>1E-4</v>
+      </c>
+      <c r="E16">
+        <v>30.025477707</v>
+      </c>
+      <c r="F16">
+        <v>47.384615384600004</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6">
+      <c r="C17">
         <v>100</v>
       </c>
-      <c r="C9" s="1">
-        <v>49.624060150399998</v>
-      </c>
-      <c r="D9" s="1">
-        <v>54.5454545455</v>
+      <c r="D17">
+        <v>0.1</v>
+      </c>
+      <c r="E17">
+        <v>40.369426751600002</v>
+      </c>
+      <c r="F17">
+        <v>48.076923076900002</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6">
+      <c r="C18">
+        <v>100</v>
+      </c>
+      <c r="D18">
+        <v>0.01</v>
+      </c>
+      <c r="E18">
+        <v>26.407643312099999</v>
+      </c>
+      <c r="F18">
+        <v>46.7692307692</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6">
+      <c r="C19">
+        <v>100</v>
+      </c>
+      <c r="D19">
+        <v>1E-3</v>
+      </c>
+      <c r="E19">
+        <v>25.605095541400001</v>
+      </c>
+      <c r="F19">
+        <v>47.7692307692</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6">
+      <c r="C20">
+        <v>100</v>
+      </c>
+      <c r="D20">
+        <v>1E-4</v>
+      </c>
+      <c r="E20">
+        <v>28.356687898099999</v>
+      </c>
+      <c r="F20">
+        <v>45.115384615400004</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6">
+      <c r="C21">
+        <v>120</v>
+      </c>
+      <c r="D21">
+        <v>0.1</v>
+      </c>
+      <c r="E21">
+        <v>40.828025477700002</v>
+      </c>
+      <c r="F21">
+        <v>50.153846153800004</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6">
+      <c r="C22">
+        <v>120</v>
+      </c>
+      <c r="D22">
+        <v>0.01</v>
+      </c>
+      <c r="E22">
+        <v>26.535031847100001</v>
+      </c>
+      <c r="F22">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6">
+      <c r="C23">
+        <v>120</v>
+      </c>
+      <c r="D23">
+        <v>1E-3</v>
+      </c>
+      <c r="E23">
+        <v>27.031847133799999</v>
+      </c>
+      <c r="F23">
+        <v>49.115384615400004</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6">
+      <c r="C24">
+        <v>120</v>
+      </c>
+      <c r="D24">
+        <v>1E-4</v>
+      </c>
+      <c r="E24">
+        <v>26.560509554100001</v>
+      </c>
+      <c r="F24">
+        <v>48.538461538500002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>